<commit_message>
address 1 2 end
</commit_message>
<xml_diff>
--- a/页面对照表.xlsx
+++ b/页面对照表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>首页</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,22 @@
   </si>
   <si>
     <t>pay-select-number.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本人收礼地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>朋友完善地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>address2.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -443,6 +459,22 @@
       </c>
       <c r="B4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>